<commit_message>
modified:   ../cam/check_C3S_atm_vars.sh modified:   postpc_clm.sh       big-fix:checkfile not defined, pointing to check_qa_start
WARNING! temporary exit before $DIR_C3S/checker_and_archive.sh
until the checker has been re-implemented
</commit_message>
<xml_diff>
--- a/src/templates/SPS4_hindcast_production_list_template.xlsx
+++ b/src/templates/SPS4_hindcast_production_list_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>start production on Zeus 14 November</t>
   </si>
@@ -54,21 +54,25 @@
     <t xml:space="preserve">hindcast list update </t>
   </si>
   <si>
-    <t>8:45 every day</t>
+    <t>9 every day</t>
   </si>
   <si>
     <t>IC CAM and NEMO update</t>
   </si>
   <si>
-    <t>18 every day</t>
+    <t>18:45 every day</t>
+  </si>
+  <si>
+    <t>core-hour cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="165" formatCode="h.mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -118,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -133,6 +137,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -391,7 +398,7 @@
       </c>
       <c r="B6" s="1">
         <f>DATEDIF( "18/11/2023",TODAY(), "D")</f>
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -462,7 +469,12 @@
       <c r="A16" s="8"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2"/>
+      <c r="A17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10">
+        <v>0.001388888888888889</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>

</xml_diff>

<commit_message>
new file:   util/copy_CamIC_from_Zeus.sh modified:   util/copy_CiceIC_to_Zeus.sh modified:   util/copy_NemoIC_to_Zeus.sh       updated and fixed procedures of exchange of ICs between Zeus and Juno
new file:   ../development_tmp/MARI/EDA_IC/nml/user_nl_clm_NoSnAg_scen
modified:   ../development_tmp/MARI/EDA_IC/nml/user_nl_datm_streams_eda_scen
        newly added namelist for CLM analysis (scenario) - still in temporary dir
</commit_message>
<xml_diff>
--- a/src/templates/SPS4_hindcast_production_list_template.xlsx
+++ b/src/templates/SPS4_hindcast_production_list_template.xlsx
@@ -36,7 +36,7 @@
     <t>days since start</t>
   </si>
   <si>
-    <t>single 6m hindcast production pace</t>
+    <t>number of single 6m hindcast produced per day</t>
   </si>
   <si>
     <t>TOTAL hindcasts to produce</t>
@@ -122,13 +122,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -398,11 +404,11 @@
       </c>
       <c r="B6" s="1">
         <f>DATEDIF( "18/11/2023",TODAY(), "D")</f>
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="7">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="str">
@@ -411,7 +417,7 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -426,7 +432,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="str">
+      <c r="B10" s="6" t="str">
         <f>CEILING(B9/B7,1)</f>
         <v>#REF!</v>
       </c>
@@ -438,41 +444,41 @@
       <c r="A12" s="2"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8">
         <v>45280.0</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="12">
         <v>0.001388888888888889</v>
       </c>
     </row>

</xml_diff>